<commit_message>
Created dimensioned parts drawing
</commit_message>
<xml_diff>
--- a/Inventory/Inventory-2013-03-07.xlsx
+++ b/Inventory/Inventory-2013-03-07.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="180" windowWidth="16275" windowHeight="7170"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="17925" windowHeight="4155"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="181">
   <si>
     <t>78-TLHR5201</t>
   </si>
@@ -370,9 +370,6 @@
     <t>72-T93YA-50K</t>
   </si>
   <si>
-    <t>Trimmer Resistors - Through Hole 3/8" SQ V/ADJ 50K</t>
-  </si>
-  <si>
     <t>696-SML-LX15IGC-TR</t>
   </si>
   <si>
@@ -536,6 +533,33 @@
   </si>
   <si>
     <t>R4</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>POT-6MM</t>
+  </si>
+  <si>
+    <t>Trimmer Resistors - Through Hole 3/8" SQ V/ADJ 50K, 19 TURN</t>
+  </si>
+  <si>
+    <t>RESON_3PIN</t>
+  </si>
+  <si>
+    <t>0201</t>
+  </si>
+  <si>
+    <t>TO-220</t>
+  </si>
+  <si>
+    <t>TO-92</t>
+  </si>
+  <si>
+    <t>DO-35</t>
   </si>
 </sst>
 </file>
@@ -594,13 +618,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,7 +940,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,24 +949,24 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="71.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>168</v>
+        <v>141</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -945,9 +980,9 @@
         <v>105</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -960,9 +995,9 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -975,9 +1010,9 @@
         <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -990,9 +1025,9 @@
         <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1005,25 +1040,25 @@
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>169</v>
+        <v>142</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1037,10 +1072,10 @@
         <v>65</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>170</v>
+        <v>142</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1054,10 +1089,10 @@
         <v>89</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>170</v>
+        <v>142</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,61 +1106,61 @@
         <v>93</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>170</v>
+        <v>142</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" s="3">
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>171</v>
+        <v>142</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" s="3">
         <v>0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>170</v>
+        <v>142</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B13" s="3">
         <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>170</v>
+        <v>142</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1139,9 +1174,9 @@
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>166</v>
+      </c>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1154,9 +1189,9 @@
         <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1169,9 +1204,9 @@
         <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -1184,9 +1219,9 @@
         <v>75</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -1199,9 +1234,9 @@
         <v>67</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>164</v>
+      </c>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1214,9 +1249,9 @@
         <v>97</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1229,9 +1264,9 @@
         <v>101</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1244,9 +1279,9 @@
         <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E21" s="1"/>
+        <v>151</v>
+      </c>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1259,9 +1294,9 @@
         <v>26</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1274,9 +1309,9 @@
         <v>61</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1289,9 +1324,9 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1304,9 +1339,9 @@
         <v>5</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>153</v>
+      </c>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1319,9 +1354,9 @@
         <v>55</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E26" s="1"/>
+        <v>149</v>
+      </c>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1334,9 +1369,9 @@
         <v>30</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E27" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
@@ -1349,9 +1384,9 @@
         <v>57</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E28" s="1"/>
+        <v>155</v>
+      </c>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -1364,9 +1399,9 @@
         <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
@@ -1379,9 +1414,9 @@
         <v>34</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E30" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -1394,9 +1429,9 @@
         <v>77</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1409,24 +1444,24 @@
         <v>73</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E32" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E33" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1439,24 +1474,24 @@
         <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E34" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E35" s="1"/>
+        <v>159</v>
+      </c>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -1469,24 +1504,24 @@
         <v>103</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E36" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B37" s="1">
         <v>6</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E37" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1499,9 +1534,9 @@
         <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E38" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1514,9 +1549,9 @@
         <v>17</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E39" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -1529,9 +1564,9 @@
         <v>79</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1544,9 +1579,9 @@
         <v>69</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E41" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -1559,9 +1594,9 @@
         <v>69</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" s="1"/>
+        <v>152</v>
+      </c>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -1574,9 +1609,9 @@
         <v>113</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E43" s="1"/>
+        <v>160</v>
+      </c>
+      <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -1589,9 +1624,9 @@
         <v>24</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E44" s="1"/>
+        <v>160</v>
+      </c>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -1604,9 +1639,9 @@
         <v>115</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E45" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1619,9 +1654,9 @@
         <v>107</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E46" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -1634,24 +1669,24 @@
         <v>38</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E47" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B48" s="3">
         <v>0</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E48" s="1"/>
+        <v>145</v>
+      </c>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
@@ -1664,10 +1699,10 @@
         <v>44</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>172</v>
+        <v>144</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1681,9 +1716,11 @@
         <v>40</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E50" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -1696,24 +1733,28 @@
         <v>81</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E51" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B52" s="1">
         <v>200</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E52" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
@@ -1726,24 +1767,28 @@
         <v>85</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E53" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B54" s="1">
         <v>100</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E54" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -1756,9 +1801,11 @@
         <v>83</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E55" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
@@ -1771,9 +1818,11 @@
         <v>91</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E56" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
@@ -1786,9 +1835,11 @@
         <v>87</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E57" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -1801,9 +1852,11 @@
         <v>51</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E58" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -1813,12 +1866,12 @@
         <v>3</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E59" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="E59" s="6"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
@@ -1831,9 +1884,11 @@
         <v>13</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E60" s="1"/>
+        <v>165</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
@@ -1846,9 +1901,9 @@
         <v>99</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E61" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
@@ -1861,9 +1916,9 @@
         <v>11</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E62" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
@@ -1876,9 +1931,9 @@
         <v>42</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E63" s="1"/>
+        <v>148</v>
+      </c>
+      <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
@@ -1891,9 +1946,9 @@
         <v>32</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E64" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="E64" s="6"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
@@ -1906,24 +1961,24 @@
         <v>19</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="E65" s="6"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B66" s="1">
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E66" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="E66" s="6"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
@@ -1936,9 +1991,11 @@
         <v>71</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E67" s="1"/>
+        <v>162</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -1951,9 +2008,11 @@
         <v>71</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E68" s="1"/>
+        <v>162</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
@@ -1966,9 +2025,11 @@
         <v>63</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E69" s="1"/>
+        <v>147</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
@@ -1981,9 +2042,11 @@
         <v>59</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E70" s="1"/>
+        <v>147</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
@@ -1996,9 +2059,11 @@
         <v>111</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E71" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
@@ -2011,9 +2076,11 @@
         <v>109</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E72" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E72">

</xml_diff>

<commit_message>
Worked on IntegTheremin and added a kiFeet utility to deal with CMP files
</commit_message>
<xml_diff>
--- a/Inventory/Inventory-2013-03-07.xlsx
+++ b/Inventory/Inventory-2013-03-07.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="17925" windowHeight="4155"/>
+    <workbookView xWindow="-15" yWindow="4200" windowWidth="17775" windowHeight="4245"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$1:$E$72</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Inventory!$A$1:$E$67</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="170">
   <si>
     <t>78-TLHR5201</t>
   </si>
@@ -403,45 +403,18 @@
     <t>Mouser Part Number</t>
   </si>
   <si>
-    <t>80-C0805C103K5R</t>
-  </si>
-  <si>
-    <t>81-GRM21BR61E475MA2L</t>
-  </si>
-  <si>
-    <t>810-C3225X5R1E106K</t>
-  </si>
-  <si>
     <t>863-MBR0530T1G</t>
   </si>
   <si>
     <t>926-LM22674MR50NOPB</t>
   </si>
   <si>
-    <t>81-GRM188R61E105KA12</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 50volts 10000pF X7R 10%</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 4.7uF 25Volts 20%</t>
-  </si>
-  <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 1210 10uF 25volts X5R 10%</t>
-  </si>
-  <si>
-    <t>Schottky Diodes &amp; Rectifiers 0.5A 30V</t>
-  </si>
-  <si>
     <t>Fixed Inductors 68uH 20%</t>
   </si>
   <si>
     <t xml:space="preserve">DC/DC Switching Converters </t>
   </si>
   <si>
-    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 1uF 25volts X5R 10%</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -523,15 +496,6 @@
     <t>Package</t>
   </si>
   <si>
-    <t>CC0603</t>
-  </si>
-  <si>
-    <t>CC0805</t>
-  </si>
-  <si>
-    <t>CC1210</t>
-  </si>
-  <si>
     <t>R4</t>
   </si>
   <si>
@@ -560,6 +524,9 @@
   </si>
   <si>
     <t>DO-35</t>
+  </si>
+  <si>
+    <t>SM0805</t>
   </si>
 </sst>
 </file>
@@ -937,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,10 +930,10 @@
         <v>125</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -980,7 +947,7 @@
         <v>105</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E2" s="6"/>
     </row>
@@ -995,7 +962,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -1010,7 +977,7 @@
         <v>48</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E4" s="6"/>
     </row>
@@ -1025,7 +992,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E5" s="6"/>
     </row>
@@ -1040,39 +1007,39 @@
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="1">
+        <v>100</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1">
         <v>100</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>169</v>
@@ -1080,16 +1047,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B9" s="1">
         <v>100</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>169</v>
@@ -1097,993 +1064,910 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>169</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>170</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="3">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="B12" s="1">
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>169</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="B13" s="1">
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>169</v>
-      </c>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="B15" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="B16" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>101</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1">
         <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1">
         <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="B27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B28" s="1">
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
+        <v>129</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="1">
-        <v>3</v>
+        <v>128</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="B32" s="1">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B33" s="3">
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="B33" s="1">
+        <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B34" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B35" s="3">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B35" s="1">
+        <v>17</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B36" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="B37" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="B38" s="1">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>16</v>
+        <v>112</v>
       </c>
       <c r="B39" s="1">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="B40" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="B41" s="1">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B42" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="B43" s="1">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B44" s="1">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="E44" s="6"/>
+        <v>135</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>114</v>
+        <v>39</v>
       </c>
       <c r="B45" s="1">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E45" s="6"/>
+        <v>135</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B46" s="1">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E46" s="6"/>
+        <v>135</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
       <c r="B47" s="1">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>38</v>
+        <v>122</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E47" s="6"/>
+        <v>135</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B48" s="3">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="B48" s="1">
+        <v>100</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E48" s="6"/>
+        <v>135</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="B49" s="1">
         <v>100</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>171</v>
+        <v>135</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="B50" s="1">
         <v>100</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>171</v>
+        <v>135</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B51" s="1">
         <v>100</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="B52" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>172</v>
+        <v>135</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B54" s="1">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>172</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="B55" s="1">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>173</v>
+        <v>156</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B56" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>172</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="E56" s="6"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="B57" s="1">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>87</v>
+        <v>11</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>172</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E57" s="6"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B58" s="1">
         <v>6</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>174</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E58" s="6"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>116</v>
+        <v>31</v>
       </c>
       <c r="B59" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>175</v>
+        <v>32</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="E59" s="6"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B60" s="1">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>176</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="E60" s="6"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="B61" s="1">
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E61" s="6"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" s="1">
         <v>10</v>
       </c>
-      <c r="B62" s="1">
-        <v>6</v>
-      </c>
       <c r="C62" s="1" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E62" s="6"/>
+        <v>153</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="B63" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E63" s="6"/>
+        <v>153</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B64" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E64" s="6"/>
+        <v>138</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="B65" s="1">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E65" s="6"/>
+        <v>138</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B66" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E66" s="6"/>
+        <v>137</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B67" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B68" s="1">
-        <v>3</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69" s="1">
-        <v>6</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B70" s="1">
-        <v>25</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B71" s="1">
-        <v>3</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B72" s="1">
-        <v>3</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>180</v>
+        <v>137</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E72">
+  <autoFilter ref="A1:E67">
     <sortState ref="A2:E72">
       <sortCondition ref="D1:D72"/>
     </sortState>

</xml_diff>